<commit_message>
Update protocol and excel
</commit_message>
<xml_diff>
--- a/PMEL OME COI PCR Protocol Sheet.xlsx
+++ b/PMEL OME COI PCR Protocol Sheet.xlsx
@@ -3,7 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="PCR Set Up" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Template Plate Layout" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sample Data Sheet Long" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="168">
   <si>
     <t>Primers: Leray CO1</t>
   </si>
@@ -22,19 +24,7 @@
     <t>Reagents</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C1 units</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C2 units</t>
-  </si>
-  <si>
-    <t>V2</t>
+    <t>Total Volume</t>
   </si>
   <si>
     <t>V1</t>
@@ -186,12 +176,354 @@
   <si>
     <t>Program:</t>
   </si>
+  <si>
+    <t>Plate Layout</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Sample 1</t>
+  </si>
+  <si>
+    <t>Sample 9</t>
+  </si>
+  <si>
+    <t>Sample 17</t>
+  </si>
+  <si>
+    <t>Sample 25</t>
+  </si>
+  <si>
+    <t>Sample 33</t>
+  </si>
+  <si>
+    <t>Sample 41</t>
+  </si>
+  <si>
+    <t>Sample 49</t>
+  </si>
+  <si>
+    <t>Sample 57</t>
+  </si>
+  <si>
+    <t>Sample 65</t>
+  </si>
+  <si>
+    <t>Sample 73</t>
+  </si>
+  <si>
+    <t>Sample 81</t>
+  </si>
+  <si>
+    <t>Sample 89</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Sample 2</t>
+  </si>
+  <si>
+    <t>Sample 10</t>
+  </si>
+  <si>
+    <t>Sample 18</t>
+  </si>
+  <si>
+    <t>Sample 26</t>
+  </si>
+  <si>
+    <t>Sample 34</t>
+  </si>
+  <si>
+    <t>Sample 42</t>
+  </si>
+  <si>
+    <t>Sample 50</t>
+  </si>
+  <si>
+    <t>Sample 58</t>
+  </si>
+  <si>
+    <t>Sample 66</t>
+  </si>
+  <si>
+    <t>Sample 74</t>
+  </si>
+  <si>
+    <t>Sample 82</t>
+  </si>
+  <si>
+    <t>Sample 90</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Sample 3</t>
+  </si>
+  <si>
+    <t>Sample 11</t>
+  </si>
+  <si>
+    <t>Sample 19</t>
+  </si>
+  <si>
+    <t>Sample 27</t>
+  </si>
+  <si>
+    <t>Sample 35</t>
+  </si>
+  <si>
+    <t>Sample 43</t>
+  </si>
+  <si>
+    <t>Sample 51</t>
+  </si>
+  <si>
+    <t>Sample 59</t>
+  </si>
+  <si>
+    <t>Sample 67</t>
+  </si>
+  <si>
+    <t>Sample 75</t>
+  </si>
+  <si>
+    <t>Sample 83</t>
+  </si>
+  <si>
+    <t>Sample 91</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Sample 4</t>
+  </si>
+  <si>
+    <t>Sample 12</t>
+  </si>
+  <si>
+    <t>Sample 20</t>
+  </si>
+  <si>
+    <t>Sample 28</t>
+  </si>
+  <si>
+    <t>Sample 36</t>
+  </si>
+  <si>
+    <t>Sample 44</t>
+  </si>
+  <si>
+    <t>Sample 52</t>
+  </si>
+  <si>
+    <t>Sample 60</t>
+  </si>
+  <si>
+    <t>Sample 68</t>
+  </si>
+  <si>
+    <t>Sample 76</t>
+  </si>
+  <si>
+    <t>Sample 84</t>
+  </si>
+  <si>
+    <t>Sample 92</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Sample 5</t>
+  </si>
+  <si>
+    <t>Sample 13</t>
+  </si>
+  <si>
+    <t>Sample 21</t>
+  </si>
+  <si>
+    <t>Sample 29</t>
+  </si>
+  <si>
+    <t>Sample 37</t>
+  </si>
+  <si>
+    <t>Sample 45</t>
+  </si>
+  <si>
+    <t>Sample 53</t>
+  </si>
+  <si>
+    <t>Sample 61</t>
+  </si>
+  <si>
+    <t>Sample 69</t>
+  </si>
+  <si>
+    <t>Sample 77</t>
+  </si>
+  <si>
+    <t>Sample 85</t>
+  </si>
+  <si>
+    <t>Sample 93</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Sample 6</t>
+  </si>
+  <si>
+    <t>Sample 14</t>
+  </si>
+  <si>
+    <t>Sample 22</t>
+  </si>
+  <si>
+    <t>Sample 30</t>
+  </si>
+  <si>
+    <t>Sample 38</t>
+  </si>
+  <si>
+    <t>Sample 46</t>
+  </si>
+  <si>
+    <t>Sample 54</t>
+  </si>
+  <si>
+    <t>Sample 62</t>
+  </si>
+  <si>
+    <t>Sample 70</t>
+  </si>
+  <si>
+    <t>Sample 78</t>
+  </si>
+  <si>
+    <t>Sample 86</t>
+  </si>
+  <si>
+    <t>Sample 94</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Sample 7</t>
+  </si>
+  <si>
+    <t>Sample 15</t>
+  </si>
+  <si>
+    <t>Sample 23</t>
+  </si>
+  <si>
+    <t>Sample 31</t>
+  </si>
+  <si>
+    <t>Sample 39</t>
+  </si>
+  <si>
+    <t>Sample 47</t>
+  </si>
+  <si>
+    <t>Sample 55</t>
+  </si>
+  <si>
+    <t>Sample 63</t>
+  </si>
+  <si>
+    <t>Sample 71</t>
+  </si>
+  <si>
+    <t>Sample 79</t>
+  </si>
+  <si>
+    <t>Sample 87</t>
+  </si>
+  <si>
+    <t>BLANK</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Sample 8</t>
+  </si>
+  <si>
+    <t>Sample 16</t>
+  </si>
+  <si>
+    <t>Sample 24</t>
+  </si>
+  <si>
+    <t>Sample 32</t>
+  </si>
+  <si>
+    <t>Sample 40</t>
+  </si>
+  <si>
+    <t>Sample 48</t>
+  </si>
+  <si>
+    <t>Sample 56</t>
+  </si>
+  <si>
+    <t>Sample 64</t>
+  </si>
+  <si>
+    <t>Sample 72</t>
+  </si>
+  <si>
+    <t>Sample 80</t>
+  </si>
+  <si>
+    <t>Sample 88</t>
+  </si>
+  <si>
+    <t>POSITIVE</t>
+  </si>
+  <si>
+    <t>Library Number</t>
+  </si>
+  <si>
+    <t>Plate Name</t>
+  </si>
+  <si>
+    <t>Plate Number</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>Metabarcoding Marker</t>
+  </si>
+  <si>
+    <t>OME P1 Sequencing MiFish</t>
+  </si>
+  <si>
+    <t>CO1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -212,8 +544,25 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +591,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FFA9D08E"/>
       </patternFill>
     </fill>
   </fills>
@@ -293,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -310,6 +677,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -322,9 +692,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -334,6 +701,9 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -381,6 +751,27 @@
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -390,6 +781,14 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -596,6 +995,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="16.5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -643,220 +1045,184 @@
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10">
+        <v>25.0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="E4" s="11">
+        <f t="shared" ref="E4:E7" si="1">D4*$G$15</f>
+        <v>1300</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="G4" s="12">
+        <f t="shared" ref="G4:G7" si="2">E4/2</f>
+        <v>650</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10">
-        <v>25.0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>12.5</v>
-      </c>
-      <c r="I4" s="11">
-        <f t="shared" ref="I4:I7" si="1">H4*$I$15</f>
-        <v>1300</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="12">
-        <f t="shared" ref="K4:K7" si="2">I4/2</f>
-        <v>650</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10">
+        <v>10</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="10">
         <v>25.0</v>
       </c>
-      <c r="H5" s="10">
+      <c r="D5" s="10">
         <v>1.0</v>
       </c>
-      <c r="I5" s="11">
+      <c r="E5" s="11">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="12">
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="12">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="10">
         <v>25.0</v>
       </c>
-      <c r="H6" s="10">
+      <c r="D6" s="10">
         <v>1.0</v>
       </c>
-      <c r="I6" s="11">
+      <c r="E6" s="11">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="12">
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="12">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10">
+        <v>14</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="10">
         <v>25.0</v>
       </c>
-      <c r="H7" s="10">
-        <f>G7-SUM(H4:H6,H8)</f>
+      <c r="D7" s="10">
+        <f>C7-SUM(D4:D6,D8)</f>
         <v>8.5</v>
       </c>
-      <c r="I7" s="11">
+      <c r="E7" s="11">
         <f t="shared" si="1"/>
         <v>884</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="12">
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="12">
         <f t="shared" si="2"/>
         <v>442</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10">
+        <v>16</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="10">
         <v>25.0</v>
       </c>
-      <c r="H8" s="10">
+      <c r="D8" s="10">
         <v>2.0</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16">
+      <c r="A9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17">
         <v>25.0</v>
       </c>
-      <c r="H9" s="16">
-        <f>SUM(H4:H8)</f>
+      <c r="D9" s="17">
+        <f>SUM(D4:D8)</f>
         <v>25</v>
       </c>
-      <c r="I9" s="16">
-        <f>SUM(I4:I8)-I8</f>
+      <c r="E9" s="17">
+        <f>SUM(E4:E8)-E8</f>
         <v>2392</v>
       </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="12">
+        <f>E9/2</f>
+        <v>1196</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="12">
-        <f>I9/2</f>
-        <v>1196</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
@@ -864,17 +1230,15 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="12">
+        <f>sum(D4:D7)</f>
+        <v>23</v>
+      </c>
       <c r="H10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="12">
-        <f>sum(H4:H7)</f>
-        <v>23</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -883,24 +1247,22 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="s">
-        <v>24</v>
+      <c r="A11" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="12">
+        <f>D8</f>
+        <v>2</v>
+      </c>
       <c r="H11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="12">
-        <f>H8</f>
-        <v>2</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -909,8 +1271,8 @@
       <c r="O11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>26</v>
+      <c r="A12" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -919,8 +1281,6 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -928,22 +1288,20 @@
       <c r="O12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="s">
-        <v>27</v>
+      <c r="A13" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="19">
+      <c r="F13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="20">
         <v>96.0</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -956,15 +1314,13 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="19">
+      <c r="F14" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="20">
         <v>8.0</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="H14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -977,16 +1333,14 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="19">
-        <f>sum(I13:I14)</f>
+      <c r="F15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="20">
+        <f>sum(G13:G14)</f>
         <v>104</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="H15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -995,10 +1349,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1016,8 +1370,8 @@
     </row>
     <row r="17">
       <c r="A17" s="2"/>
-      <c r="B17" s="6" t="s">
-        <v>33</v>
+      <c r="B17" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1051,8 +1405,8 @@
       <c r="O18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="20" t="s">
-        <v>34</v>
+      <c r="A19" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1071,7 +1425,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1090,16 +1444,16 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1114,14 +1468,14 @@
       <c r="O21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="22">
+      <c r="A22" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="23">
         <v>95.0</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>41</v>
+      <c r="C22" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="D22" s="10">
         <v>1.0</v>
@@ -1139,16 +1493,16 @@
       <c r="O22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="25">
+      <c r="A23" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="26">
         <v>16.0</v>
       </c>
       <c r="E23" s="2"/>
@@ -1164,17 +1518,17 @@
       <c r="O23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>48</v>
+      <c r="A24" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>44</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1189,16 +1543,16 @@
       <c r="O24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="9"/>
+      <c r="A25" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="14"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1212,16 +1566,16 @@
       <c r="O25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="25">
+      <c r="A26" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="26">
         <v>25.0</v>
       </c>
       <c r="E26" s="2"/>
@@ -1237,16 +1591,16 @@
       <c r="O26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="28"/>
+      <c r="A27" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="29"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1260,16 +1614,16 @@
       <c r="O27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="9"/>
+      <c r="A28" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="14"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1283,14 +1637,14 @@
       <c r="O28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="22">
+      <c r="A29" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="23">
         <v>72.0</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>41</v>
+      <c r="C29" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="D29" s="10">
         <v>1.0</v>
@@ -1308,14 +1662,14 @@
       <c r="O29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="22">
+      <c r="A30" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="23">
         <v>4.0</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>55</v>
+      <c r="C30" s="23" t="s">
+        <v>51</v>
       </c>
       <c r="D30" s="10">
         <v>1.0</v>
@@ -1334,7 +1688,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1353,7 +1707,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -17829,4 +18183,2637 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="31">
+        <v>3.0</v>
+      </c>
+      <c r="E3" s="31">
+        <v>4.0</v>
+      </c>
+      <c r="F3" s="31">
+        <v>5.0</v>
+      </c>
+      <c r="G3" s="31">
+        <v>6.0</v>
+      </c>
+      <c r="H3" s="31">
+        <v>7.0</v>
+      </c>
+      <c r="I3" s="31">
+        <v>8.0</v>
+      </c>
+      <c r="J3" s="31">
+        <v>9.0</v>
+      </c>
+      <c r="K3" s="31">
+        <v>10.0</v>
+      </c>
+      <c r="L3" s="31">
+        <v>11.0</v>
+      </c>
+      <c r="M3" s="31">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="M10" s="33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M11" s="34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="25.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="12">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="12">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="12">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="12">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="12">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D19" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="12">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="12">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="12">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="12">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="12">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="12">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="12">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="12">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D29" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="12">
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D30" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="12">
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D31" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="12">
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D32" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="12">
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D33" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="G33" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="12">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D34" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="12">
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D35" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="12">
+        <v>35.0</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D36" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="12">
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D37" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="12">
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D38" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="12">
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D39" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="12">
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D40" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="12">
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D41" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="G41" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="12">
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D42" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="12">
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D43" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="12">
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D44" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="12">
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D45" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G45" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="12">
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C46" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D46" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="12">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D47" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="12">
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D48" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="G48" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="12">
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D49" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="G49" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="12">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D50" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="12">
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D51" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="12">
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D52" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="12">
+        <v>52.0</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D53" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="G53" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="12">
+        <v>53.0</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C54" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D54" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="12">
+        <v>54.0</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D55" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="12">
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D56" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="G56" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="12">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C57" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D57" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="G57" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="12">
+        <v>57.0</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D58" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G58" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="12">
+        <v>58.0</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C59" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D59" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G59" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="12">
+        <v>59.0</v>
+      </c>
+      <c r="B60" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D60" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="G60" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="12">
+        <v>60.0</v>
+      </c>
+      <c r="B61" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C61" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D61" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="G61" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="12">
+        <v>61.0</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C62" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D62" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="G62" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="12">
+        <v>62.0</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D63" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="12">
+        <v>63.0</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C64" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D64" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F64" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="12">
+        <v>64.0</v>
+      </c>
+      <c r="B65" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D65" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="G65" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="12">
+        <v>65.0</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D66" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F66" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="G66" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="12">
+        <v>66.0</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D67" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F67" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="G67" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="12">
+        <v>67.0</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C68" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D68" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G68" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="12">
+        <v>68.0</v>
+      </c>
+      <c r="B69" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C69" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D69" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G69" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="12">
+        <v>69.0</v>
+      </c>
+      <c r="B70" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C70" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D70" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="G70" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="12">
+        <v>70.0</v>
+      </c>
+      <c r="B71" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D71" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G71" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="12">
+        <v>71.0</v>
+      </c>
+      <c r="B72" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D72" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="12">
+        <v>72.0</v>
+      </c>
+      <c r="B73" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D73" s="12">
+        <v>9.0</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F73" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="G73" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="12">
+        <v>73.0</v>
+      </c>
+      <c r="B74" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D74" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F74" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G74" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="12">
+        <v>74.0</v>
+      </c>
+      <c r="B75" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C75" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D75" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F75" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G75" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="12">
+        <v>75.0</v>
+      </c>
+      <c r="B76" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D76" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F76" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G76" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="12">
+        <v>76.0</v>
+      </c>
+      <c r="B77" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C77" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D77" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F77" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G77" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="12">
+        <v>77.0</v>
+      </c>
+      <c r="B78" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D78" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G78" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="12">
+        <v>78.0</v>
+      </c>
+      <c r="B79" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C79" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D79" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="G79" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="12">
+        <v>79.0</v>
+      </c>
+      <c r="B80" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D80" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F80" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G80" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="12">
+        <v>80.0</v>
+      </c>
+      <c r="B81" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D81" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="G81" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="12">
+        <v>81.0</v>
+      </c>
+      <c r="B82" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C82" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D82" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G82" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="12">
+        <v>82.0</v>
+      </c>
+      <c r="B83" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D83" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F83" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G83" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="12">
+        <v>83.0</v>
+      </c>
+      <c r="B84" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C84" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D84" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F84" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G84" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="12">
+        <v>84.0</v>
+      </c>
+      <c r="B85" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C85" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D85" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F85" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G85" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="12">
+        <v>85.0</v>
+      </c>
+      <c r="B86" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C86" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D86" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F86" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G86" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="12">
+        <v>86.0</v>
+      </c>
+      <c r="B87" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D87" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F87" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="G87" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="12">
+        <v>87.0</v>
+      </c>
+      <c r="B88" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C88" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D88" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F88" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G88" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="12">
+        <v>88.0</v>
+      </c>
+      <c r="B89" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D89" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F89" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="G89" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="12">
+        <v>89.0</v>
+      </c>
+      <c r="B90" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C90" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D90" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F90" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G90" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="12">
+        <v>90.0</v>
+      </c>
+      <c r="B91" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C91" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D91" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F91" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="G91" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="12">
+        <v>91.0</v>
+      </c>
+      <c r="B92" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C92" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D92" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F92" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="G92" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="12">
+        <v>92.0</v>
+      </c>
+      <c r="B93" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C93" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D93" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F93" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="G93" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="12">
+        <v>93.0</v>
+      </c>
+      <c r="B94" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C94" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D94" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F94" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G94" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="12">
+        <v>94.0</v>
+      </c>
+      <c r="B95" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C95" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D95" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F95" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="G95" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="12">
+        <v>95.0</v>
+      </c>
+      <c r="B96" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C96" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D96" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F96" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="G96" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="12">
+        <v>96.0</v>
+      </c>
+      <c r="B97" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C97" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D97" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F97" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="G97" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>